<commit_message>
Commit for Minor correction in files
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/4U3I1U3I3I.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/4U3I1U3I3I.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7669830-A244-4001-BA37-00C4FC63E579}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9985B289-C478-4DD4-8F87-1181CAF8DD30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -416,7 +416,7 @@
     <t>DSP_2_Feeder_Map_2</t>
   </si>
   <si>
-    <t>Cabling 4U3U3I3I3I</t>
+    <t>Cabling 3U4U3I3I3I</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1577,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1649,7 +1649,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -1996,8 +1996,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2117,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,13 +2139,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,13 +2153,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,13 +2167,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>